<commit_message>
Added localStorage for saving state
</commit_message>
<xml_diff>
--- a/Google Analytics Sample - Oct 13, 2017.xlsx
+++ b/Google Analytics Sample - Oct 13, 2017.xlsx
@@ -1,14 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27931"/>
+  <workbookPr autoCompressPictures="0"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15620" tabRatio="500" activeTab="1"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Summary" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="Dataset1" sheetId="2" r:id="rId4"/>
-    <sheet state="visible" name="Dataset2" sheetId="3" r:id="rId5"/>
+    <sheet name="Summary" sheetId="1" r:id="rId1"/>
+    <sheet name="Dataset1" sheetId="2" r:id="rId2"/>
+    <sheet name="Dataset2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -93,11 +101,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="12.0"/>
-      <name val="Arial"/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
       <family val="1"/>
       <scheme val="minor"/>
     </font>
@@ -107,7 +123,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -119,58 +135,410 @@
       <diagonal/>
     </border>
   </borders>
+  <cellStyleXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="2" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="10" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="14" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium4" defaultTableStyle="TableStyleMedium9"/>
+  <cellStyles count="4">
+    <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row>
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row>
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row>
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row/>
-    <row>
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row>
+    <row r="6" spans="1:1">
       <c r="A6" t="str">
         <f>HYPERLINK("#'Dataset1'!A1", "Dataset1")</f>
-      </c>
-    </row>
-    <row>
+        <v>Dataset1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
       <c r="A7" t="str">
         <f>HYPERLINK("#'Dataset2'!A1", "Dataset2")</f>
+        <v>Dataset2</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row>
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -202,21 +570,21 @@
         <v>13</v>
       </c>
     </row>
-    <row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="C2" s="2">
-        <v>0.6521739130434783</v>
+        <v>0.65217391304347827</v>
       </c>
       <c r="D2">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="E2" s="2">
-        <v>0.8695652173913043</v>
+        <v>0.86956521739130432</v>
       </c>
       <c r="F2" s="1">
         <v>1.1304347826086956</v>
@@ -225,27 +593,27 @@
         <v>59.391304347826086</v>
       </c>
       <c r="H2" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J2" s="1">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2">
         <v>0.5714285714285714</v>
       </c>
       <c r="D3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E3" s="2">
         <v>0.8571428571428571</v>
@@ -257,27 +625,27 @@
         <v>18.857142857142858</v>
       </c>
       <c r="H3" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J3" s="1">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>16</v>
       </c>
       <c r="B4">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="E4" s="2">
         <v>0.8</v>
@@ -289,27 +657,27 @@
         <v>29.2</v>
       </c>
       <c r="H4" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J4" s="1">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>17</v>
       </c>
       <c r="B5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C5" s="2">
         <v>0.25</v>
       </c>
       <c r="D5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="2">
         <v>0.5</v>
@@ -321,219 +689,219 @@
         <v>460.75</v>
       </c>
       <c r="H5" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J5" s="1">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>18</v>
       </c>
       <c r="B6">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C6" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="E6" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H6" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J6" s="1">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>19</v>
       </c>
       <c r="B7">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C7" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E7" s="2">
-        <v>0.6666666666666666</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F7" s="1">
         <v>2.3333333333333335</v>
       </c>
       <c r="G7" s="1">
-        <v>523.0</v>
+        <v>523</v>
       </c>
       <c r="H7" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J7" s="1">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>20</v>
       </c>
       <c r="B8">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C8" s="2">
-        <v>0.6666666666666666</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D8">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E8" s="2">
-        <v>0.6666666666666666</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F8" s="1">
         <v>1.3333333333333333</v>
       </c>
       <c r="G8" s="1">
-        <v>276.3333333333333</v>
+        <v>276.33333333333331</v>
       </c>
       <c r="H8" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J8" s="1">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>21</v>
       </c>
       <c r="B9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C9" s="2">
         <v>0.5</v>
       </c>
       <c r="D9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H9" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J9" s="1">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>22</v>
       </c>
       <c r="B10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H10" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I10">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J10" s="1">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>23</v>
       </c>
       <c r="B11">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E11" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G11" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H11" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I11">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J11" s="1">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="B12">
-        <v>61.0</v>
+        <v>61</v>
       </c>
       <c r="C12" s="2">
-        <v>0.639344262295082</v>
+        <v>0.63934426229508201</v>
       </c>
       <c r="D12">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="E12" s="2">
-        <v>0.8524590163934426</v>
+        <v>0.85245901639344257</v>
       </c>
       <c r="F12" s="1">
         <v>1.3114754098360655</v>
@@ -542,23 +910,35 @@
         <v>96.47540983606558</v>
       </c>
       <c r="H12" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I12">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J12" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row>
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -566,67 +946,73 @@
         <v>5</v>
       </c>
     </row>
-    <row>
+    <row r="2" spans="1:2">
       <c r="A2" s="3">
         <v>43014</v>
       </c>
       <c r="B2">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="3">
         <v>43015</v>
       </c>
       <c r="B3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="3">
         <v>43016</v>
       </c>
       <c r="B4">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="3">
         <v>43017</v>
       </c>
       <c r="B5">
-        <v>16.0</v>
-      </c>
-    </row>
-    <row>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" s="3">
         <v>43018</v>
       </c>
       <c r="B6">
-        <v>14.0</v>
-      </c>
-    </row>
-    <row>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" s="3">
         <v>43019</v>
       </c>
       <c r="B7">
-        <v>9.0</v>
-      </c>
-    </row>
-    <row>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" s="3">
         <v>43020</v>
       </c>
       <c r="B8">
-        <v>14.0</v>
-      </c>
-    </row>
-    <row>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="B9">
-        <v>61.0</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>